<commit_message>
Atualização automática de URUGUAIANA.xlsx
</commit_message>
<xml_diff>
--- a/URUGUAIANA.xlsx
+++ b/URUGUAIANA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FF3B1CF-D341-4308-B2BC-1BE95EB8DCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FB17F81-D261-42B9-AAE4-E704CF8C91B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1244,7 +1244,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{A316D7CC-980D-4392-91EB-A6A184CDA34D}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{16C24597-15BA-4C1F-B332-E14758A2531E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1274,10 +1274,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A84F6382-7B6A-4E25-B76E-5CB946569609}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38827D62-934C-4C0D-A3F8-04186DEC0148}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1315,7 +1315,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FD37C90-A379-42EF-8F0A-E9AF4EB4E77C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1B16F8D-333C-424C-BA57-5E3A1DDD17B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1378,7 +1378,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21C4D5C3-19FB-4052-B3AD-E890E75AD6FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{401422D1-055E-47F9-B3B3-3165EF23064A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1397,7 +1397,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA406843-53EC-6440-443F-3328850528C9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D03CE3E-46DE-3AF7-C72A-78A56E2CD286}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1446,7 +1446,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2563BE1D-A816-D7F9-5613-81F7097B8F4C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17F57983-2429-CCFF-3B67-FDBFC947C26B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1465,7 +1465,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{580F8F0B-B224-51F7-7FE2-65BCEC713F76}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E01EB88C-DB3E-3DA4-AE47-1EB301A2E2A7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1496,7 +1496,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D905F432-A2F9-2393-0AD8-C0F9ED7E1774}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DCB7869-AE4E-9E7F-21FC-E25099E2AF5D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1527,7 +1527,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0E5D857-D859-98F9-10E4-202BAB83CDB9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A3655C4-6514-9972-0BB0-170311D8C699}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1570,7 +1570,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{811573DB-AD71-433B-9D96-9F359B1E2F1E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C07C452A-E173-42E0-9612-BFFAB29D12BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1608,7 +1608,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA69007E-4B36-43FE-AB97-0FD0FBBEB808}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB0B8361-8C8B-474A-98DF-0566139F5AB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1651,7 +1651,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0810FBC9-BE03-46DF-8FC2-4515B87CCA1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91ABBD5E-2780-4761-A22B-0BE0D53E0A30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1964,7 +1964,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA008B8-620C-4532-BA69-F1228E4151D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5893C75-3EA8-4BB3-8B47-7D9CE6E2E78C}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>